<commit_message>
update and new data
</commit_message>
<xml_diff>
--- a/input/urbanrural.xlsx
+++ b/input/urbanrural.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$D$2099</definedName>
     <definedName name="gem_20150501">#REF!</definedName>
-    <definedName name="STAT_UR_TYPOLOGIE_GEM">data!$A$1:$D$2126</definedName>
+    <definedName name="STAT_UR_TYPOLOGIE_GEM">data!$A$1:$D$2128</definedName>
     <definedName name="typologie_gem_201505">#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10603" uniqueCount="4240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10611" uniqueCount="4242">
   <si>
     <t>Tourismus</t>
   </si>
@@ -12754,13 +12754,19 @@
   </si>
   <si>
     <t>Peuerbach/Grieskirchen</t>
+  </si>
+  <si>
+    <t>Favoriten</t>
+  </si>
+  <si>
+    <t>Brigittenau</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -12787,6 +12793,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -12808,11 +12820,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -13382,10 +13395,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2119"/>
+  <dimension ref="A1:F2121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1258" workbookViewId="0">
-      <selection activeCell="B1283" sqref="B1283"/>
+    <sheetView tabSelected="1" topLeftCell="A2086" workbookViewId="0">
+      <selection activeCell="D2108" sqref="D2108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -55535,11 +55548,11 @@
       </c>
     </row>
     <row r="2108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2108" s="2">
-        <v>91101</v>
+      <c r="A2108" s="4">
+        <v>91001</v>
       </c>
       <c r="B2108" s="2" t="s">
-        <v>4227</v>
+        <v>4240</v>
       </c>
       <c r="C2108">
         <v>101</v>
@@ -55556,10 +55569,10 @@
     </row>
     <row r="2109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2109" s="2">
-        <v>91201</v>
+        <v>91101</v>
       </c>
       <c r="B2109" s="2" t="s">
-        <v>4228</v>
+        <v>4227</v>
       </c>
       <c r="C2109">
         <v>101</v>
@@ -55576,10 +55589,10 @@
     </row>
     <row r="2110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2110" s="2">
-        <v>91301</v>
+        <v>91201</v>
       </c>
       <c r="B2110" s="2" t="s">
-        <v>4229</v>
+        <v>4228</v>
       </c>
       <c r="C2110">
         <v>101</v>
@@ -55596,10 +55609,10 @@
     </row>
     <row r="2111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2111" s="2">
-        <v>91401</v>
+        <v>91301</v>
       </c>
       <c r="B2111" s="2" t="s">
-        <v>4230</v>
+        <v>4229</v>
       </c>
       <c r="C2111">
         <v>101</v>
@@ -55616,10 +55629,10 @@
     </row>
     <row r="2112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2112" s="2">
-        <v>91501</v>
+        <v>91401</v>
       </c>
       <c r="B2112" s="2" t="s">
-        <v>4231</v>
+        <v>4230</v>
       </c>
       <c r="C2112">
         <v>101</v>
@@ -55636,10 +55649,10 @@
     </row>
     <row r="2113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2113" s="2">
-        <v>91601</v>
+        <v>91501</v>
       </c>
       <c r="B2113" s="2" t="s">
-        <v>4232</v>
+        <v>4231</v>
       </c>
       <c r="C2113">
         <v>101</v>
@@ -55656,10 +55669,10 @@
     </row>
     <row r="2114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2114" s="2">
-        <v>91701</v>
+        <v>91601</v>
       </c>
       <c r="B2114" s="2" t="s">
-        <v>4233</v>
+        <v>4232</v>
       </c>
       <c r="C2114">
         <v>101</v>
@@ -55676,10 +55689,10 @@
     </row>
     <row r="2115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2115" s="2">
-        <v>91801</v>
+        <v>91701</v>
       </c>
       <c r="B2115" s="2" t="s">
-        <v>4234</v>
+        <v>4233</v>
       </c>
       <c r="C2115">
         <v>101</v>
@@ -55696,10 +55709,10 @@
     </row>
     <row r="2116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2116" s="2">
-        <v>91901</v>
+        <v>91801</v>
       </c>
       <c r="B2116" s="2" t="s">
-        <v>4235</v>
+        <v>4234</v>
       </c>
       <c r="C2116">
         <v>101</v>
@@ -55716,10 +55729,10 @@
     </row>
     <row r="2117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2117" s="2">
-        <v>92101</v>
+        <v>91901</v>
       </c>
       <c r="B2117" s="2" t="s">
-        <v>4236</v>
+        <v>4235</v>
       </c>
       <c r="C2117">
         <v>101</v>
@@ -55736,10 +55749,10 @@
     </row>
     <row r="2118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2118" s="2">
-        <v>92201</v>
+        <v>92001</v>
       </c>
       <c r="B2118" s="2" t="s">
-        <v>4237</v>
+        <v>4241</v>
       </c>
       <c r="C2118">
         <v>101</v>
@@ -55756,10 +55769,10 @@
     </row>
     <row r="2119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2119" s="2">
-        <v>92301</v>
+        <v>92101</v>
       </c>
       <c r="B2119" s="2" t="s">
-        <v>4238</v>
+        <v>4236</v>
       </c>
       <c r="C2119">
         <v>101</v>
@@ -55771,6 +55784,46 @@
         <v>4192</v>
       </c>
       <c r="F2119" t="s">
+        <v>4193</v>
+      </c>
+    </row>
+    <row r="2120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2120" s="2">
+        <v>92201</v>
+      </c>
+      <c r="B2120" s="2" t="s">
+        <v>4237</v>
+      </c>
+      <c r="C2120">
+        <v>101</v>
+      </c>
+      <c r="D2120" t="s">
+        <v>4214</v>
+      </c>
+      <c r="E2120" t="s">
+        <v>4192</v>
+      </c>
+      <c r="F2120" t="s">
+        <v>4193</v>
+      </c>
+    </row>
+    <row r="2121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2121" s="2">
+        <v>92301</v>
+      </c>
+      <c r="B2121" s="2" t="s">
+        <v>4238</v>
+      </c>
+      <c r="C2121">
+        <v>101</v>
+      </c>
+      <c r="D2121" t="s">
+        <v>4214</v>
+      </c>
+      <c r="E2121" t="s">
+        <v>4192</v>
+      </c>
+      <c r="F2121" t="s">
         <v>4193</v>
       </c>
     </row>

</xml_diff>